<commit_message>
Updated server code and orders.xlsx
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -397,157 +397,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>orderId</v>
+        <v>S.No</v>
       </c>
       <c r="B1" t="str">
-        <v>name</v>
+        <v>Date</v>
       </c>
       <c r="C1" t="str">
-        <v>email</v>
+        <v>Name</v>
       </c>
       <c r="D1" t="str">
-        <v>phone</v>
+        <v>Item</v>
       </c>
       <c r="E1" t="str">
-        <v>address</v>
+        <v>Quantity</v>
       </c>
       <c r="F1" t="str">
-        <v>persons</v>
+        <v>Amount</v>
       </c>
       <c r="G1" t="str">
-        <v>items</v>
+        <v>Ph no</v>
       </c>
       <c r="H1" t="str">
-        <v>total</v>
+        <v>Tracking ID</v>
       </c>
       <c r="I1" t="str">
-        <v>payment</v>
+        <v>Order Status</v>
       </c>
       <c r="J1" t="str">
-        <v>status</v>
-      </c>
-      <c r="K1" t="str">
-        <v>createdAt</v>
-      </c>
-      <c r="L1" t="str">
-        <v>destLat</v>
-      </c>
-      <c r="M1" t="str">
-        <v>destLon</v>
-      </c>
-      <c r="N1" t="str">
-        <v>gmail</v>
-      </c>
-      <c r="O1" t="str">
-        <v>timestamp</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="str">
-        <v>SK1760293451353</v>
-      </c>
-      <c r="B2" t="str">
-        <v>hs</v>
-      </c>
-      <c r="C2" t="str">
-        <v>9909846152@gmail.com</v>
-      </c>
-      <c r="D2" t="str">
-        <v>srht</v>
-      </c>
-      <c r="E2" t="str">
-        <v>srh</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2" t="str">
-        <v>[{"name":"Chicken Pickle 100g","price":100,"qty":2}]</v>
-      </c>
-      <c r="H2">
-        <v>200</v>
-      </c>
-      <c r="I2" t="str">
-        <v>Cash on Delivery</v>
-      </c>
-      <c r="J2" t="str">
-        <v>Accepted</v>
-      </c>
-      <c r="K2" t="str">
-        <v>2025-10-12T18:24:13.031Z</v>
-      </c>
-      <c r="L2">
-        <v>18.5950634</v>
-      </c>
-      <c r="M2">
-        <v>73.7306531</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>1760296039158</v>
-      </c>
-      <c r="B3" t="str">
-        <v>yfhght</v>
-      </c>
-      <c r="D3" t="str">
-        <v>687697687</v>
-      </c>
-      <c r="E3" t="str">
-        <v>jyhfulyflyfkhg</v>
-      </c>
-      <c r="F3" t="str">
-        <v>9</v>
-      </c>
-      <c r="J3" t="str">
-        <v>Preparing</v>
-      </c>
-      <c r="N3" t="str">
-        <v>gfgfd@gmail.com</v>
-      </c>
-      <c r="O3" t="str">
-        <v>13/10/2025, 12:37:19 am</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>1760297417363</v>
-      </c>
-      <c r="B4" t="str">
-        <v>Shaik Imambasha</v>
-      </c>
-      <c r="D4" t="str">
-        <v>85858</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Jayammacoloy,Bakarapuram</v>
-      </c>
-      <c r="F4" t="str">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>300</v>
-      </c>
-      <c r="J4" t="str">
-        <v>Delivered</v>
-      </c>
-      <c r="N4" t="str">
-        <v>gfgfd@gmail.com</v>
-      </c>
-      <c r="O4" t="str">
-        <v>13/10/2025, 1:00:17 am</v>
+        <v>Timestamp</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:O4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>